<commit_message>
Fixed % variation issue (-lag) Fixed usa gdp_index mistype Fixed data uploading system
</commit_message>
<xml_diff>
--- a/DATA/actind.xlsx
+++ b/DATA/actind.xlsx
@@ -5,8 +5,8 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Tabulado" sheetId="1" r:id="Rffb90d8258594b1e"/>
-    <sheet name="MetaInfo" sheetId="2" r:id="Re92bb4a2c5ce4f52"/>
+    <sheet name="Tabulado" sheetId="1" r:id="R92687ce5ed144914"/>
+    <sheet name="MetaInfo" sheetId="2" r:id="R322b4027472b4191"/>
   </sheets>
 </workbook>
 </file>
@@ -24,7 +24,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">R. Cifras revisadas</t>
+          <t xml:space="preserve">P. Cifras preliminares</t>
         </d:r>
       </text>
     </comment>
@@ -35,7 +35,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">R. Cifras revisadas</t>
+          <t xml:space="preserve">P. Cifras preliminares</t>
         </d:r>
       </text>
     </comment>
@@ -46,7 +46,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">R. Cifras revisadas</t>
+          <t xml:space="preserve">P. Cifras preliminares</t>
         </d:r>
       </text>
     </comment>
@@ -57,11 +57,22 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
+          <t xml:space="preserve">P. Cifras preliminares</t>
+        </d:r>
+      </text>
+    </comment>
+    <comment ref="ND6" authorId="0">
+      <text>
+        <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+          </rPr>
           <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
-    <comment ref="ND6" authorId="0">
+    <comment ref="NE6" authorId="0">
       <text>
         <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
           <rPr>
@@ -82,7 +93,7 @@
     <t>Instituto Nacional de Estadística y Geografía (INEGI).</t>
   </si>
   <si>
-    <t>Sistema de Cuentas Nacionales de México. Indicador Mensual de la Actividad Industrial. Año Base 2013. Serie de enero de 1993 a marzo de 2021</t>
+    <t>Sistema de Cuentas Nacionales de México. Indicador Mensual de la Actividad Industrial. Año Base 2013. Serie de enero de 1993 a abril de 2021</t>
   </si>
   <si>
     <t>Índice de volumen físico base 2013=100</t>
@@ -185,7 +196,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">R</d:t>
+      <d:t xml:space="preserve">P</d:t>
     </d:r>
   </si>
   <si>
@@ -205,7 +216,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">R</d:t>
+      <d:t xml:space="preserve">P</d:t>
     </d:r>
   </si>
   <si>
@@ -267,7 +278,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">R</d:t>
+      <d:t xml:space="preserve">P</d:t>
     </d:r>
   </si>
   <si>
@@ -287,6 +298,26 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
+      <d:t xml:space="preserve">P</d:t>
+    </d:r>
+  </si>
+  <si>
+    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:rPr>
+        <d:b/>
+        <d:sz val="10"/>
+        <d:rFont val="Calibri"/>
+      </d:rPr>
+      <d:t> Marzo</d:t>
+    </d:r>
+    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:rPr>
+        <d:b/>
+        <d:vertAlign val="superscript"/>
+        <d:sz val="11"/>
+        <d:color rgb="FF000000"/>
+        <d:rFont val="Arial"/>
+      </d:rPr>
       <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
@@ -297,7 +328,7 @@
         <d:sz val="10"/>
         <d:rFont val="Calibri"/>
       </d:rPr>
-      <d:t> Marzo</d:t>
+      <d:t> Abril</d:t>
     </d:r>
     <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <d:rPr>
@@ -423,25 +454,6 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t>R</d:t>
-    </d:r>
-    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <d:rPr>
-        <d:sz val="10"/>
-        <d:color rgb="FF000000"/>
-        <d:rFont val="Arial"/>
-      </d:rPr>
-      <d:t xml:space="preserve">Cifras revisadas</d:t>
-    </d:r>
-  </si>
-  <si>
-    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <d:rPr>
-        <d:vertAlign val="superscript"/>
-        <d:sz val="11"/>
-        <d:color rgb="FF000000"/>
-        <d:rFont val="Arial"/>
-      </d:rPr>
       <d:t>P</d:t>
     </d:r>
     <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
@@ -454,7 +466,23 @@
     </d:r>
   </si>
   <si>
-    <t>Nota: Con base en los ´´Lineamientos de cambios a la información divulgada en las publicaciones estadísticas y geográficas del INEGI´´ y que complementan la ´´Normas Especiales para la Divulgación de Datos´´ del FMI, al disponer de un dato más reciente generado por las Cuentas de Bienes y Servicios 2019 versión revisada y en esta ocasión, por la incorporación de la construcción del Aeropuerto Internacional Felipe Ángeles a la Encuesta Nacional de Empresas Constructoras (ENEC), desde octubre 2019, así como la inclusión de la última información estadística disponible de la Encuesta Mensual de la Industria Manufacturera y de los registros administrativos, se debe realizar la actualización de este indicador. Como resultado de incorporar dicha información, se identifican diferencias en los niveles de los índices y variaciones que fueron oportunamente publicadas.</t>
+    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:rPr>
+        <d:vertAlign val="superscript"/>
+        <d:sz val="11"/>
+        <d:color rgb="FF000000"/>
+        <d:rFont val="Arial"/>
+      </d:rPr>
+      <d:t>R</d:t>
+    </d:r>
+    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:rPr>
+        <d:sz val="10"/>
+        <d:color rgb="FF000000"/>
+        <d:rFont val="Arial"/>
+      </d:rPr>
+      <d:t xml:space="preserve">Cifras revisadas</d:t>
+    </d:r>
   </si>
   <si>
     <t>Fuente: INEGI. Sistema de Cuentas Nacionales de México. Indicador Mensual de la Actividad Industrial</t>
@@ -523,19 +551,19 @@
     <t>COBERTURA TEMPORAL</t>
   </si>
   <si>
-    <t>1993-01-2021-03</t>
+    <t>1993-01-2021-04</t>
   </si>
   <si>
     <t>DESCRIPCIÓN PERIODO</t>
   </si>
   <si>
-    <t>Serie de enero de 1993 a marzo de 2021</t>
+    <t>Serie de enero de 1993 a abril de 2021</t>
   </si>
   <si>
     <t>FECHA DE ACTUALIZACIÓN</t>
   </si>
   <si>
-    <t>2021-05-12</t>
+    <t>2021-06-11</t>
   </si>
 </sst>
 </file>
@@ -676,7 +704,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:NN48"/>
+  <dimension ref="A1:NN47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2621,7 +2649,7 @@
         <v>48</v>
       </c>
       <c r="NE6" s="10" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="NF6" s="10" t="s">
         <v>37</v>
@@ -2653,7 +2681,7 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" s="11">
         <v>69.222752741001</v>
@@ -3754,42 +3782,42 @@
         <v>95.077009216112</v>
       </c>
       <c r="ND7" s="11">
-        <v>101.161517771466</v>
-      </c>
-      <c r="NE7" s="14" t="s">
-        <v>50</v>
+        <v>101.173294574985</v>
+      </c>
+      <c r="NE7" s="11">
+        <v>97.035755126306</v>
       </c>
       <c r="NF7" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG7" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH7" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI7" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ7" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK7" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL7" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM7" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN7" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8" s="12">
         <v>85.987958716261</v>
@@ -4890,42 +4918,42 @@
         <v>73.158130206302</v>
       </c>
       <c r="ND8" s="12">
-        <v>75.513000327488</v>
-      </c>
-      <c r="NE8" s="15" t="s">
-        <v>50</v>
+        <v>75.491659482618</v>
+      </c>
+      <c r="NE8" s="12">
+        <v>72.812366103638</v>
       </c>
       <c r="NF8" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG8" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH8" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI8" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ8" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK8" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL8" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM8" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN8" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" s="11">
         <v>99.519341749343</v>
@@ -6028,40 +6056,40 @@
       <c r="ND9" s="11">
         <v>69.239305126376</v>
       </c>
-      <c r="NE9" s="14" t="s">
-        <v>50</v>
+      <c r="NE9" s="11">
+        <v>66.960931086384</v>
       </c>
       <c r="NF9" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG9" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH9" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI9" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ9" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK9" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL9" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM9" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN9" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" s="12">
         <v>48.814950253715</v>
@@ -7162,42 +7190,42 @@
         <v>104.923635255705</v>
       </c>
       <c r="ND10" s="12">
-        <v>106.044719883642</v>
-      </c>
-      <c r="NE10" s="15" t="s">
-        <v>50</v>
+        <v>105.898530626126</v>
+      </c>
+      <c r="NE10" s="12">
+        <v>103.648086907926</v>
       </c>
       <c r="NF10" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG10" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH10" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI10" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ10" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK10" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL10" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM10" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN10" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B11" s="11">
         <v>22.744141472693</v>
@@ -8300,40 +8328,40 @@
       <c r="ND11" s="11">
         <v>80.522360035365</v>
       </c>
-      <c r="NE11" s="14" t="s">
-        <v>50</v>
+      <c r="NE11" s="11">
+        <v>73.171197853963</v>
       </c>
       <c r="NF11" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG11" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH11" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI11" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ11" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK11" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL11" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM11" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN11" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B12" s="12">
         <v>38.665943249786</v>
@@ -8858,7 +8886,7 @@
         <v>82.285700021575</v>
       </c>
       <c r="FT12" s="12">
-        <v>84.872908092727</v>
+        <v>84.872908092728</v>
       </c>
       <c r="FU12" s="12">
         <v>87.006771936463</v>
@@ -9434,42 +9462,42 @@
         <v>96.753802086374</v>
       </c>
       <c r="ND12" s="12">
-        <v>104.27279060218</v>
-      </c>
-      <c r="NE12" s="15" t="s">
-        <v>50</v>
+        <v>104.373253704486</v>
+      </c>
+      <c r="NE12" s="12">
+        <v>105.395835417527</v>
       </c>
       <c r="NF12" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG12" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH12" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI12" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ12" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK12" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL12" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM12" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN12" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B13" s="11">
         <v>33.532463105934</v>
@@ -9994,7 +10022,7 @@
         <v>77.96308232892</v>
       </c>
       <c r="FT13" s="11">
-        <v>81.350354205881</v>
+        <v>81.350354205882</v>
       </c>
       <c r="FU13" s="11">
         <v>83.983953249091</v>
@@ -10570,42 +10598,42 @@
         <v>94.871791910574</v>
       </c>
       <c r="ND13" s="11">
-        <v>103.871447565443</v>
-      </c>
-      <c r="NE13" s="14" t="s">
-        <v>50</v>
+        <v>104.001169619886</v>
+      </c>
+      <c r="NE13" s="11">
+        <v>105.019732238922</v>
       </c>
       <c r="NF13" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG13" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH13" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI13" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ13" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK13" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL13" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM13" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN13" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B14" s="12">
         <v>56.292184219235</v>
@@ -11708,40 +11736,40 @@
       <c r="ND14" s="12">
         <v>105.650836075953</v>
       </c>
-      <c r="NE14" s="15" t="s">
-        <v>50</v>
+      <c r="NE14" s="12">
+        <v>106.687217690315</v>
       </c>
       <c r="NF14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" s="11">
         <v>71.2627077305</v>
@@ -12842,42 +12870,42 @@
         <v>95.591974437701</v>
       </c>
       <c r="ND15" s="11">
-        <v>89.900801958986</v>
-      </c>
-      <c r="NE15" s="14" t="s">
-        <v>50</v>
+        <v>89.819049902068</v>
+      </c>
+      <c r="NE15" s="11">
+        <v>89.325076023488</v>
       </c>
       <c r="NF15" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG15" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH15" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI15" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ15" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK15" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL15" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM15" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN15" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B16" s="12">
         <v>84.037802362945</v>
@@ -13771,7 +13799,7 @@
         <v>107.456876229305</v>
       </c>
       <c r="KM16" s="12">
-        <v>109.69972489064</v>
+        <v>109.699724890639</v>
       </c>
       <c r="KN16" s="12">
         <v>106.221231756916</v>
@@ -13978,42 +14006,42 @@
         <v>105.535413256398</v>
       </c>
       <c r="ND16" s="12">
-        <v>93.346027093119</v>
-      </c>
-      <c r="NE16" s="15" t="s">
-        <v>50</v>
+        <v>93.208922854422</v>
+      </c>
+      <c r="NE16" s="12">
+        <v>92.907420756914</v>
       </c>
       <c r="NF16" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG16" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH16" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI16" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ16" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK16" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL16" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM16" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN16" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" s="11">
         <v>35.064527007042</v>
@@ -15090,7 +15118,7 @@
         <v>50.631944025606</v>
       </c>
       <c r="MV17" s="11">
-        <v>56.073389775793</v>
+        <v>56.073389775792</v>
       </c>
       <c r="MW17" s="11">
         <v>53.730057240421</v>
@@ -15114,42 +15142,42 @@
         <v>51.957028028674</v>
       </c>
       <c r="ND17" s="11">
-        <v>58.258313926902</v>
-      </c>
-      <c r="NE17" s="14" t="s">
-        <v>50</v>
+        <v>58.177850195742</v>
+      </c>
+      <c r="NE17" s="11">
+        <v>53.952265709705</v>
       </c>
       <c r="NF17" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG17" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH17" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI17" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ17" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK17" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL17" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM17" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN17" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B18" s="12">
         <v>73.87209194618</v>
@@ -16250,42 +16278,42 @@
         <v>131.628084968613</v>
       </c>
       <c r="ND18" s="12">
-        <v>138.730974722543</v>
-      </c>
-      <c r="NE18" s="15" t="s">
-        <v>50</v>
+        <v>138.980055867861</v>
+      </c>
+      <c r="NE18" s="12">
+        <v>145.533594665284</v>
       </c>
       <c r="NF18" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG18" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH18" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI18" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ18" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK18" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL18" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM18" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN18" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B19" s="11">
         <v>63.653052579688</v>
@@ -17122,7 +17150,7 @@
         <v>106.941322006685</v>
       </c>
       <c r="JT19" s="11">
-        <v>105.230620689974</v>
+        <v>105.230620689975</v>
       </c>
       <c r="JU19" s="11">
         <v>105.554969592329</v>
@@ -17170,7 +17198,7 @@
         <v>107.711396263853</v>
       </c>
       <c r="KJ19" s="11">
-        <v>108.022283783149</v>
+        <v>108.022283783148</v>
       </c>
       <c r="KK19" s="11">
         <v>113.751953282089</v>
@@ -17386,42 +17414,42 @@
         <v>104.488403384241</v>
       </c>
       <c r="ND19" s="11">
-        <v>117.639028669979</v>
-      </c>
-      <c r="NE19" s="14" t="s">
-        <v>50</v>
+        <v>117.701173217825</v>
+      </c>
+      <c r="NE19" s="11">
+        <v>110.710380245816</v>
       </c>
       <c r="NF19" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG19" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH19" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI19" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ19" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK19" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL19" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM19" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN19" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B20" s="12">
         <v>63.907698868213</v>
@@ -18522,42 +18550,42 @@
         <v>113.620995092318</v>
       </c>
       <c r="ND20" s="12">
-        <v>119.905062245519</v>
-      </c>
-      <c r="NE20" s="15" t="s">
-        <v>50</v>
+        <v>120.003149176838</v>
+      </c>
+      <c r="NE20" s="12">
+        <v>115.96336718697</v>
       </c>
       <c r="NF20" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG20" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH20" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI20" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ20" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK20" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL20" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM20" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN20" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B21" s="11">
         <v>56.569385260854</v>
@@ -19658,42 +19686,42 @@
         <v>107.897779664634</v>
       </c>
       <c r="ND21" s="11">
-        <v>125.926238854996</v>
-      </c>
-      <c r="NE21" s="14" t="s">
-        <v>50</v>
+        <v>125.927442997954</v>
+      </c>
+      <c r="NE21" s="11">
+        <v>126.713582958041</v>
       </c>
       <c r="NF21" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG21" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH21" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI21" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ21" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK21" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL21" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM21" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN21" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B22" s="12">
         <v>114.319677175604</v>
@@ -20119,7 +20147,7 @@
         <v>117.907452401807</v>
       </c>
       <c r="EM22" s="12">
-        <v>102.663934277922</v>
+        <v>102.663934277921</v>
       </c>
       <c r="EN22" s="12">
         <v>121.171668236243</v>
@@ -20257,7 +20285,7 @@
         <v>110.759665886981</v>
       </c>
       <c r="GG22" s="12">
-        <v>117.713454149937</v>
+        <v>117.713454149938</v>
       </c>
       <c r="GH22" s="12">
         <v>117.736921541804</v>
@@ -20794,42 +20822,42 @@
         <v>81.34647735232</v>
       </c>
       <c r="ND22" s="12">
-        <v>88.981329939774</v>
-      </c>
-      <c r="NE22" s="15" t="s">
-        <v>50</v>
+        <v>89.01383173174</v>
+      </c>
+      <c r="NE22" s="12">
+        <v>88.384684308811</v>
       </c>
       <c r="NF22" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG22" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH22" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI22" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ22" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK22" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL22" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM22" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN22" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B23" s="11">
         <v>120.050850501477</v>
@@ -21549,7 +21577,7 @@
         <v>93.175225480757</v>
       </c>
       <c r="IG23" s="11">
-        <v>96.070279662976</v>
+        <v>96.070279662975</v>
       </c>
       <c r="IH23" s="11">
         <v>101.737313361619</v>
@@ -21930,42 +21958,42 @@
         <v>102.970780477154</v>
       </c>
       <c r="ND23" s="11">
-        <v>116.369200776183</v>
-      </c>
-      <c r="NE23" s="14" t="s">
-        <v>50</v>
+        <v>116.221712292736</v>
+      </c>
+      <c r="NE23" s="11">
+        <v>87.79525425784</v>
       </c>
       <c r="NF23" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG23" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH23" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI23" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ23" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK23" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL23" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM23" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN23" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B24" s="12">
         <v>90.688383871069</v>
@@ -23066,42 +23094,42 @@
         <v>68.789347704684</v>
       </c>
       <c r="ND24" s="12">
-        <v>83.42370030114</v>
-      </c>
-      <c r="NE24" s="15" t="s">
-        <v>50</v>
+        <v>83.459645534257</v>
+      </c>
+      <c r="NE24" s="12">
+        <v>77.584071509803</v>
       </c>
       <c r="NF24" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG24" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH24" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI24" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ24" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK24" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL24" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM24" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN24" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B25" s="11">
         <v>139.460849924193</v>
@@ -24202,42 +24230,42 @@
         <v>71.093476954908</v>
       </c>
       <c r="ND25" s="11">
-        <v>73.932529219672</v>
-      </c>
-      <c r="NE25" s="14" t="s">
-        <v>50</v>
+        <v>73.936166356142</v>
+      </c>
+      <c r="NE25" s="11">
+        <v>69.734921214659</v>
       </c>
       <c r="NF25" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG25" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH25" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI25" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ25" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK25" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL25" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM25" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN25" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B26" s="12">
         <v>130.395494603712</v>
@@ -24999,7 +25027,7 @@
         <v>111.318450734813</v>
       </c>
       <c r="IU26" s="12">
-        <v>97.416158126745</v>
+        <v>97.416158126744</v>
       </c>
       <c r="IV26" s="12">
         <v>107.114454959646</v>
@@ -25338,42 +25366,42 @@
         <v>94.46006993351</v>
       </c>
       <c r="ND26" s="12">
-        <v>100.811856472554</v>
-      </c>
-      <c r="NE26" s="15" t="s">
-        <v>50</v>
+        <v>101.229662444775</v>
+      </c>
+      <c r="NE26" s="12">
+        <v>91.750667075691</v>
       </c>
       <c r="NF26" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG26" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH26" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI26" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ26" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK26" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL26" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM26" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN26" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B27" s="11">
         <v>51.479382699588</v>
@@ -26474,42 +26502,42 @@
         <v>107.645840337483</v>
       </c>
       <c r="ND27" s="11">
-        <v>122.146207939647</v>
-      </c>
-      <c r="NE27" s="14" t="s">
-        <v>50</v>
+        <v>122.145350408347</v>
+      </c>
+      <c r="NE27" s="11">
+        <v>130.972043021847</v>
       </c>
       <c r="NF27" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG27" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH27" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI27" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ27" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK27" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL27" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM27" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN27" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B28" s="12">
         <v>68.358361009475</v>
@@ -27610,42 +27638,42 @@
         <v>92.050810458411</v>
       </c>
       <c r="ND28" s="12">
-        <v>101.019369152552</v>
-      </c>
-      <c r="NE28" s="15" t="s">
-        <v>50</v>
+        <v>101.013238804924</v>
+      </c>
+      <c r="NE28" s="12">
+        <v>70.802412138902</v>
       </c>
       <c r="NF28" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG28" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH28" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI28" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ28" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK28" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL28" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM28" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN28" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B29" s="11">
         <v>76.901717312341</v>
@@ -28748,40 +28776,40 @@
       <c r="ND29" s="11">
         <v>65.118064062477</v>
       </c>
-      <c r="NE29" s="14" t="s">
-        <v>50</v>
+      <c r="NE29" s="11">
+        <v>48.969382478693</v>
       </c>
       <c r="NF29" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG29" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH29" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI29" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ29" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK29" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL29" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM29" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN29" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B30" s="12">
         <v>73.778714563351</v>
@@ -29882,42 +29910,42 @@
         <v>75.628031858608</v>
       </c>
       <c r="ND30" s="12">
-        <v>82.058849013869</v>
-      </c>
-      <c r="NE30" s="15" t="s">
-        <v>50</v>
+        <v>82.052720546437</v>
+      </c>
+      <c r="NE30" s="12">
+        <v>77.431767017449</v>
       </c>
       <c r="NF30" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG30" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH30" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI30" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ30" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK30" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL30" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM30" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN30" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B31" s="11">
         <v>73.811018646336</v>
@@ -30100,7 +30128,7 @@
         <v>92.530672204995</v>
       </c>
       <c r="BJ31" s="11">
-        <v>84.822315953758</v>
+        <v>84.822315953759</v>
       </c>
       <c r="BK31" s="11">
         <v>91.197770456276</v>
@@ -30721,7 +30749,7 @@
         <v>105.279540530588</v>
       </c>
       <c r="JI31" s="11">
-        <v>103.79997342929</v>
+        <v>103.799973429289</v>
       </c>
       <c r="JJ31" s="11">
         <v>97.719773098197</v>
@@ -31018,42 +31046,42 @@
         <v>116.921893537868</v>
       </c>
       <c r="ND31" s="11">
-        <v>123.808961321331</v>
-      </c>
-      <c r="NE31" s="14" t="s">
-        <v>50</v>
+        <v>123.930523132745</v>
+      </c>
+      <c r="NE31" s="11">
+        <v>126.591375619751</v>
       </c>
       <c r="NF31" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG31" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH31" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI31" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ31" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK31" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL31" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM31" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN31" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B32" s="12">
         <v>86.120032958035</v>
@@ -32154,42 +32182,42 @@
         <v>109.385968935807</v>
       </c>
       <c r="ND32" s="12">
-        <v>120.83492059761</v>
-      </c>
-      <c r="NE32" s="15" t="s">
-        <v>50</v>
+        <v>120.846536399751</v>
+      </c>
+      <c r="NE32" s="12">
+        <v>114.47289932209</v>
       </c>
       <c r="NF32" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG32" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH32" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI32" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ32" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK32" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL32" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM32" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN32" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B33" s="11">
         <v>69.399412813085</v>
@@ -33290,42 +33318,42 @@
         <v>93.401841438228</v>
       </c>
       <c r="ND33" s="11">
-        <v>102.737305035994</v>
-      </c>
-      <c r="NE33" s="14" t="s">
-        <v>50</v>
+        <v>102.843824222956</v>
+      </c>
+      <c r="NE33" s="11">
+        <v>99.360726982542</v>
       </c>
       <c r="NF33" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG33" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH33" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI33" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ33" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK33" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL33" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM33" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN33" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B34" s="12">
         <v>72.622901666126</v>
@@ -33898,7 +33926,7 @@
         <v>116.458896659146</v>
       </c>
       <c r="GJ34" s="12">
-        <v>107.179010492019</v>
+        <v>107.179010492018</v>
       </c>
       <c r="GK34" s="12">
         <v>115.46329954894</v>
@@ -33937,7 +33965,7 @@
         <v>107.220124251125</v>
       </c>
       <c r="GW34" s="12">
-        <v>105.452330853942</v>
+        <v>105.452330853943</v>
       </c>
       <c r="GX34" s="12">
         <v>115.02590334585</v>
@@ -34129,7 +34157,7 @@
         <v>101.595831692184</v>
       </c>
       <c r="JI34" s="12">
-        <v>101.467953672713</v>
+        <v>101.467953672712</v>
       </c>
       <c r="JJ34" s="12">
         <v>97.944257143157</v>
@@ -34225,7 +34253,7 @@
         <v>109.976767217928</v>
       </c>
       <c r="KO34" s="12">
-        <v>107.874867879491</v>
+        <v>107.87486787949</v>
       </c>
       <c r="KP34" s="12">
         <v>112.689978501788</v>
@@ -34426,42 +34454,42 @@
         <v>103.013107508299</v>
       </c>
       <c r="ND34" s="12">
-        <v>123.944196369126</v>
-      </c>
-      <c r="NE34" s="15" t="s">
-        <v>50</v>
+        <v>124.059377651231</v>
+      </c>
+      <c r="NE34" s="12">
+        <v>110.683830820724</v>
       </c>
       <c r="NF34" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG34" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH34" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI34" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ34" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK34" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL34" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM34" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN34" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B35" s="11">
         <v>60.182989506094</v>
@@ -35562,42 +35590,42 @@
         <v>95.197274496333</v>
       </c>
       <c r="ND35" s="11">
-        <v>116.165328027052</v>
-      </c>
-      <c r="NE35" s="14" t="s">
-        <v>50</v>
+        <v>116.593168105942</v>
+      </c>
+      <c r="NE35" s="11">
+        <v>109.847219655183</v>
       </c>
       <c r="NF35" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG35" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH35" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI35" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ35" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK35" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL35" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM35" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN35" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B36" s="12">
         <v>61.132998870046</v>
@@ -36167,7 +36195,7 @@
         <v>107.863814613867</v>
       </c>
       <c r="GI36" s="12">
-        <v>126.09453857615</v>
+        <v>126.094538576149</v>
       </c>
       <c r="GJ36" s="12">
         <v>125.489105446636</v>
@@ -36188,7 +36216,7 @@
         <v>112.53675029352</v>
       </c>
       <c r="GP36" s="12">
-        <v>105.708098106801</v>
+        <v>105.708098106802</v>
       </c>
       <c r="GQ36" s="12">
         <v>110.211745409613</v>
@@ -36698,42 +36726,42 @@
         <v>138.106003815529</v>
       </c>
       <c r="ND36" s="12">
-        <v>151.886459216485</v>
-      </c>
-      <c r="NE36" s="15" t="s">
-        <v>50</v>
+        <v>151.886953168357</v>
+      </c>
+      <c r="NE36" s="12">
+        <v>139.395620149147</v>
       </c>
       <c r="NF36" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG36" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH36" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI36" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ36" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK36" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL36" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM36" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN36" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B37" s="11">
         <v>65.758484330262</v>
@@ -37132,7 +37160,7 @@
         <v>109.375136947249</v>
       </c>
       <c r="ED37" s="11">
-        <v>103.630122854371</v>
+        <v>103.630122854372</v>
       </c>
       <c r="EE37" s="11">
         <v>95.918036976017</v>
@@ -37519,7 +37547,7 @@
         <v>100.808222495904</v>
       </c>
       <c r="JC37" s="11">
-        <v>98.353856914581</v>
+        <v>98.35385691458</v>
       </c>
       <c r="JD37" s="11">
         <v>94.616077569601</v>
@@ -37711,7 +37739,7 @@
         <v>117.339402188725</v>
       </c>
       <c r="LO37" s="11">
-        <v>111.243619478106</v>
+        <v>111.243619478105</v>
       </c>
       <c r="LP37" s="11">
         <v>113.05386535961</v>
@@ -37834,42 +37862,42 @@
         <v>125.544060627645</v>
       </c>
       <c r="ND37" s="11">
-        <v>141.408539119876</v>
-      </c>
-      <c r="NE37" s="14" t="s">
-        <v>50</v>
+        <v>141.407793014073</v>
+      </c>
+      <c r="NE37" s="11">
+        <v>139.180788588841</v>
       </c>
       <c r="NF37" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG37" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH37" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI37" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ37" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK37" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL37" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM37" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN37" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="12">
         <v>33.546378018984</v>
@@ -38970,42 +38998,42 @@
         <v>112.89850566318</v>
       </c>
       <c r="ND38" s="12">
-        <v>139.337814937628</v>
-      </c>
-      <c r="NE38" s="15" t="s">
-        <v>50</v>
+        <v>139.354329819995</v>
+      </c>
+      <c r="NE38" s="12">
+        <v>126.44222991451</v>
       </c>
       <c r="NF38" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG38" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH38" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI38" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ38" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK38" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL38" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM38" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN38" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B39" s="11">
         <v>113.328554079414</v>
@@ -39965,7 +39993,7 @@
         <v>88.455549785448</v>
       </c>
       <c r="LI39" s="11">
-        <v>90.391653887423</v>
+        <v>90.391653887422</v>
       </c>
       <c r="LJ39" s="11">
         <v>94.579359088044</v>
@@ -40106,42 +40134,42 @@
         <v>91.384697857615</v>
       </c>
       <c r="ND39" s="11">
-        <v>93.716300135205</v>
-      </c>
-      <c r="NE39" s="14" t="s">
-        <v>50</v>
+        <v>93.717052700775</v>
+      </c>
+      <c r="NE39" s="11">
+        <v>72.589839628819</v>
       </c>
       <c r="NF39" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG39" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH39" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI39" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ39" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK39" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL39" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM39" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN39" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B40" s="12">
         <v>42.404526159595</v>
@@ -40948,7 +40976,7 @@
         <v>100.047769469755</v>
       </c>
       <c r="JJ40" s="12">
-        <v>98.265948470573</v>
+        <v>98.265948470574</v>
       </c>
       <c r="JK40" s="12">
         <v>111.175398244536</v>
@@ -41242,61 +41270,56 @@
         <v>120.145900102462</v>
       </c>
       <c r="ND40" s="12">
-        <v>125.211642172008</v>
-      </c>
-      <c r="NE40" s="15" t="s">
-        <v>50</v>
+        <v>125.213406415957</v>
+      </c>
+      <c r="NE40" s="12">
+        <v>115.330289807305</v>
       </c>
       <c r="NF40" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NG40" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NH40" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NI40" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NJ40" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NK40" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NL40" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NM40" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="NN40" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="3"/>
+      <c r="A47" s="3"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -41332,7 +41355,7 @@
     <mergeCell ref="A5:A6"/>
   </mergeCells>
   <headerFooter/>
-  <legacyDrawing r:id="Ra356858bdb6f4d9e"/>
+  <legacyDrawing r:id="Rd5a862cd3f9a4e26"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
database update added USA unemp level
</commit_message>
<xml_diff>
--- a/DATA/actind.xlsx
+++ b/DATA/actind.xlsx
@@ -5,8 +5,8 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Tabulado" sheetId="1" r:id="R92687ce5ed144914"/>
-    <sheet name="MetaInfo" sheetId="2" r:id="R322b4027472b4191"/>
+    <sheet name="Tabulado" sheetId="1" r:id="R4c21679cfce54f6d"/>
+    <sheet name="MetaInfo" sheetId="2" r:id="R9444480f536d4e9d"/>
   </sheets>
 </workbook>
 </file>
@@ -68,11 +68,22 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
+          <t xml:space="preserve">P. Cifras preliminares</t>
+        </d:r>
+      </text>
+    </comment>
+    <comment ref="NE6" authorId="0">
+      <text>
+        <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+          </rPr>
           <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
-    <comment ref="NE6" authorId="0">
+    <comment ref="NF6" authorId="0">
       <text>
         <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
           <rPr>
@@ -88,12 +99,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>Instituto Nacional de Estadística y Geografía (INEGI).</t>
   </si>
   <si>
-    <t>Sistema de Cuentas Nacionales de México. Indicador Mensual de la Actividad Industrial. Año Base 2013. Serie de enero de 1993 a abril de 2021</t>
+    <t>Sistema de Cuentas Nacionales de México. Indicador Mensual de la Actividad Industrial. Año Base 2013. Serie de enero de 1993 a mayo de 2021</t>
   </si>
   <si>
     <t>Índice de volumen físico base 2013=100</t>
@@ -318,6 +329,26 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
+      <d:t xml:space="preserve">P</d:t>
+    </d:r>
+  </si>
+  <si>
+    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:rPr>
+        <d:b/>
+        <d:sz val="10"/>
+        <d:rFont val="Calibri"/>
+      </d:rPr>
+      <d:t> Abril</d:t>
+    </d:r>
+    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:rPr>
+        <d:b/>
+        <d:vertAlign val="superscript"/>
+        <d:sz val="11"/>
+        <d:color rgb="FF000000"/>
+        <d:rFont val="Arial"/>
+      </d:rPr>
       <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
@@ -328,7 +359,7 @@
         <d:sz val="10"/>
         <d:rFont val="Calibri"/>
       </d:rPr>
-      <d:t> Abril</d:t>
+      <d:t> Mayo</d:t>
     </d:r>
     <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <d:rPr>
@@ -551,19 +582,19 @@
     <t>COBERTURA TEMPORAL</t>
   </si>
   <si>
-    <t>1993-01-2021-04</t>
+    <t>1993-01-2021-05</t>
   </si>
   <si>
     <t>DESCRIPCIÓN PERIODO</t>
   </si>
   <si>
-    <t>Serie de enero de 1993 a abril de 2021</t>
+    <t>Serie de enero de 1993 a mayo de 2021</t>
   </si>
   <si>
     <t>FECHA DE ACTUALIZACIÓN</t>
   </si>
   <si>
-    <t>2021-06-11</t>
+    <t>2021-07-12</t>
   </si>
 </sst>
 </file>
@@ -2652,7 +2683,7 @@
         <v>49</v>
       </c>
       <c r="NF6" s="10" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="NG6" s="10" t="s">
         <v>38</v>
@@ -2681,7 +2712,7 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7" s="11">
         <v>69.222752741001</v>
@@ -3785,39 +3816,39 @@
         <v>101.173294574985</v>
       </c>
       <c r="NE7" s="11">
-        <v>97.035755126306</v>
-      </c>
-      <c r="NF7" s="14" t="s">
-        <v>51</v>
+        <v>96.974394088319</v>
+      </c>
+      <c r="NF7" s="11">
+        <v>98.584005227973</v>
       </c>
       <c r="NG7" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH7" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI7" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ7" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK7" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL7" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM7" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN7" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8" s="12">
         <v>85.987958716261</v>
@@ -4921,39 +4952,39 @@
         <v>75.491659482618</v>
       </c>
       <c r="NE8" s="12">
-        <v>72.812366103638</v>
-      </c>
-      <c r="NF8" s="15" t="s">
-        <v>51</v>
+        <v>72.599022127376</v>
+      </c>
+      <c r="NF8" s="12">
+        <v>75.933525075631</v>
       </c>
       <c r="NG8" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH8" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI8" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ8" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK8" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL8" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM8" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN8" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" s="11">
         <v>99.519341749343</v>
@@ -6059,37 +6090,37 @@
       <c r="NE9" s="11">
         <v>66.960931086384</v>
       </c>
-      <c r="NF9" s="14" t="s">
-        <v>51</v>
+      <c r="NF9" s="11">
+        <v>68.745850557353</v>
       </c>
       <c r="NG9" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH9" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI9" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ9" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK9" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL9" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM9" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN9" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B10" s="12">
         <v>48.814950253715</v>
@@ -7193,39 +7224,39 @@
         <v>105.898530626126</v>
       </c>
       <c r="NE10" s="12">
-        <v>103.648086907926</v>
-      </c>
-      <c r="NF10" s="15" t="s">
-        <v>51</v>
+        <v>102.237651496025</v>
+      </c>
+      <c r="NF10" s="12">
+        <v>106.679779663612</v>
       </c>
       <c r="NG10" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH10" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI10" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ10" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK10" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL10" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM10" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN10" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" s="11">
         <v>22.744141472693</v>
@@ -8329,39 +8360,39 @@
         <v>80.522360035365</v>
       </c>
       <c r="NE11" s="11">
-        <v>73.171197853963</v>
-      </c>
-      <c r="NF11" s="14" t="s">
-        <v>51</v>
+        <v>73.077916740191</v>
+      </c>
+      <c r="NF11" s="11">
+        <v>89.413487904052</v>
       </c>
       <c r="NG11" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH11" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI11" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ11" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK11" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL11" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM11" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN11" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B12" s="12">
         <v>38.665943249786</v>
@@ -9465,39 +9496,39 @@
         <v>104.373253704486</v>
       </c>
       <c r="NE12" s="12">
-        <v>105.395835417527</v>
-      </c>
-      <c r="NF12" s="15" t="s">
-        <v>51</v>
+        <v>105.702109260093</v>
+      </c>
+      <c r="NF12" s="12">
+        <v>112.470678968301</v>
       </c>
       <c r="NG12" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH12" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI12" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ12" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK12" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL12" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM12" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN12" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13" s="11">
         <v>33.532463105934</v>
@@ -10601,39 +10632,39 @@
         <v>104.001169619886</v>
       </c>
       <c r="NE13" s="11">
-        <v>105.019732238922</v>
-      </c>
-      <c r="NF13" s="14" t="s">
-        <v>51</v>
+        <v>105.415205513864</v>
+      </c>
+      <c r="NF13" s="11">
+        <v>113.78478279497</v>
       </c>
       <c r="NG13" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH13" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI13" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ13" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK13" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL13" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM13" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN13" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B14" s="12">
         <v>56.292184219235</v>
@@ -11739,37 +11770,37 @@
       <c r="NE14" s="12">
         <v>106.687217690315</v>
       </c>
-      <c r="NF14" s="15" t="s">
-        <v>51</v>
+      <c r="NF14" s="12">
+        <v>107.958591639886</v>
       </c>
       <c r="NG14" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH14" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI14" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ14" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK14" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL14" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM14" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN14" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B15" s="11">
         <v>71.2627077305</v>
@@ -12873,39 +12904,39 @@
         <v>89.819049902068</v>
       </c>
       <c r="NE15" s="11">
-        <v>89.325076023488</v>
-      </c>
-      <c r="NF15" s="14" t="s">
-        <v>51</v>
+        <v>89.208788073416</v>
+      </c>
+      <c r="NF15" s="11">
+        <v>90.189061761914</v>
       </c>
       <c r="NG15" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH15" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI15" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ15" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK15" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL15" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM15" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN15" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B16" s="12">
         <v>84.037802362945</v>
@@ -14009,39 +14040,39 @@
         <v>93.208922854422</v>
       </c>
       <c r="NE16" s="12">
-        <v>92.907420756914</v>
-      </c>
-      <c r="NF16" s="15" t="s">
-        <v>51</v>
+        <v>92.754632831593</v>
+      </c>
+      <c r="NF16" s="12">
+        <v>99.441211250345</v>
       </c>
       <c r="NG16" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH16" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI16" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ16" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK16" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL16" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM16" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN16" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B17" s="11">
         <v>35.064527007042</v>
@@ -15145,39 +15176,39 @@
         <v>58.177850195742</v>
       </c>
       <c r="NE17" s="11">
-        <v>53.952265709705</v>
-      </c>
-      <c r="NF17" s="14" t="s">
-        <v>51</v>
+        <v>53.932911021137</v>
+      </c>
+      <c r="NF17" s="11">
+        <v>52.169258900858</v>
       </c>
       <c r="NG17" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH17" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI17" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ17" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK17" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL17" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM17" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN17" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B18" s="12">
         <v>73.87209194618</v>
@@ -16281,39 +16312,39 @@
         <v>138.980055867861</v>
       </c>
       <c r="NE18" s="12">
-        <v>145.533594665284</v>
-      </c>
-      <c r="NF18" s="15" t="s">
-        <v>51</v>
+        <v>145.42412467361</v>
+      </c>
+      <c r="NF18" s="12">
+        <v>118.041701958256</v>
       </c>
       <c r="NG18" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH18" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI18" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ18" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK18" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL18" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM18" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN18" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B19" s="11">
         <v>63.653052579688</v>
@@ -17417,39 +17448,39 @@
         <v>117.701173217825</v>
       </c>
       <c r="NE19" s="11">
-        <v>110.710380245816</v>
-      </c>
-      <c r="NF19" s="14" t="s">
-        <v>51</v>
+        <v>110.708045467409</v>
+      </c>
+      <c r="NF19" s="11">
+        <v>111.352612395082</v>
       </c>
       <c r="NG19" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH19" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI19" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ19" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK19" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL19" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM19" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN19" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" s="12">
         <v>63.907698868213</v>
@@ -18553,39 +18584,39 @@
         <v>120.003149176838</v>
       </c>
       <c r="NE20" s="12">
-        <v>115.96336718697</v>
-      </c>
-      <c r="NF20" s="15" t="s">
-        <v>51</v>
+        <v>116.028216694837</v>
+      </c>
+      <c r="NF20" s="12">
+        <v>117.271714519741</v>
       </c>
       <c r="NG20" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH20" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI20" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ20" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK20" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL20" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM20" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN20" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B21" s="11">
         <v>56.569385260854</v>
@@ -19689,39 +19720,39 @@
         <v>125.927442997954</v>
       </c>
       <c r="NE21" s="11">
-        <v>126.713582958041</v>
-      </c>
-      <c r="NF21" s="14" t="s">
-        <v>51</v>
+        <v>126.713701134469</v>
+      </c>
+      <c r="NF21" s="11">
+        <v>130.981819887064</v>
       </c>
       <c r="NG21" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH21" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI21" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ21" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK21" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL21" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM21" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN21" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B22" s="12">
         <v>114.319677175604</v>
@@ -20825,39 +20856,39 @@
         <v>89.01383173174</v>
       </c>
       <c r="NE22" s="12">
-        <v>88.384684308811</v>
-      </c>
-      <c r="NF22" s="15" t="s">
-        <v>51</v>
+        <v>88.310669607533</v>
+      </c>
+      <c r="NF22" s="12">
+        <v>92.519890605507</v>
       </c>
       <c r="NG22" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH22" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI22" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ22" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK22" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL22" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM22" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN22" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B23" s="11">
         <v>120.050850501477</v>
@@ -21961,39 +21992,39 @@
         <v>116.221712292736</v>
       </c>
       <c r="NE23" s="11">
-        <v>87.79525425784</v>
-      </c>
-      <c r="NF23" s="14" t="s">
-        <v>51</v>
+        <v>87.834547805602</v>
+      </c>
+      <c r="NF23" s="11">
+        <v>103.940790203397</v>
       </c>
       <c r="NG23" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH23" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI23" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ23" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK23" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL23" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM23" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN23" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B24" s="12">
         <v>90.688383871069</v>
@@ -23097,39 +23128,39 @@
         <v>83.459645534257</v>
       </c>
       <c r="NE24" s="12">
-        <v>77.584071509803</v>
-      </c>
-      <c r="NF24" s="15" t="s">
-        <v>51</v>
+        <v>77.634937095721</v>
+      </c>
+      <c r="NF24" s="12">
+        <v>84.370726712106</v>
       </c>
       <c r="NG24" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH24" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI24" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ24" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK24" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL24" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM24" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN24" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B25" s="11">
         <v>139.460849924193</v>
@@ -23186,7 +23217,7 @@
         <v>137.73392677423</v>
       </c>
       <c r="T25" s="11">
-        <v>144.853523451828</v>
+        <v>144.853523451829</v>
       </c>
       <c r="U25" s="11">
         <v>125.678147001672</v>
@@ -24233,39 +24264,39 @@
         <v>73.936166356142</v>
       </c>
       <c r="NE25" s="11">
-        <v>69.734921214659</v>
-      </c>
-      <c r="NF25" s="14" t="s">
-        <v>51</v>
+        <v>69.716039984756</v>
+      </c>
+      <c r="NF25" s="11">
+        <v>71.392662888295</v>
       </c>
       <c r="NG25" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH25" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI25" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ25" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK25" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL25" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM25" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN25" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B26" s="12">
         <v>130.395494603712</v>
@@ -25369,39 +25400,39 @@
         <v>101.229662444775</v>
       </c>
       <c r="NE26" s="12">
-        <v>91.750667075691</v>
-      </c>
-      <c r="NF26" s="15" t="s">
-        <v>51</v>
+        <v>91.740052830419</v>
+      </c>
+      <c r="NF26" s="12">
+        <v>94.792114198158</v>
       </c>
       <c r="NG26" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH26" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI26" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ26" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK26" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL26" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM26" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN26" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B27" s="11">
         <v>51.479382699588</v>
@@ -25467,7 +25498,7 @@
         <v>58.165535087493</v>
       </c>
       <c r="W27" s="11">
-        <v>56.147613112816</v>
+        <v>56.147613112815</v>
       </c>
       <c r="X27" s="11">
         <v>58.778310292597</v>
@@ -26505,39 +26536,39 @@
         <v>122.145350408347</v>
       </c>
       <c r="NE27" s="11">
-        <v>130.972043021847</v>
-      </c>
-      <c r="NF27" s="14" t="s">
-        <v>51</v>
+        <v>130.961845217912</v>
+      </c>
+      <c r="NF27" s="11">
+        <v>131.038768287143</v>
       </c>
       <c r="NG27" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH27" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI27" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ27" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK27" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL27" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM27" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN27" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B28" s="12">
         <v>68.358361009475</v>
@@ -26822,7 +26853,7 @@
         <v>103.154618627309</v>
       </c>
       <c r="CR28" s="12">
-        <v>76.513206616607</v>
+        <v>76.513206616608</v>
       </c>
       <c r="CS28" s="12">
         <v>110.768147030929</v>
@@ -27641,39 +27672,39 @@
         <v>101.013238804924</v>
       </c>
       <c r="NE28" s="12">
-        <v>70.802412138902</v>
-      </c>
-      <c r="NF28" s="15" t="s">
-        <v>51</v>
+        <v>70.818178121182</v>
+      </c>
+      <c r="NF28" s="12">
+        <v>101.6639671821</v>
       </c>
       <c r="NG28" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH28" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI28" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ28" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK28" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL28" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM28" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN28" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B29" s="11">
         <v>76.901717312341</v>
@@ -28779,37 +28810,37 @@
       <c r="NE29" s="11">
         <v>48.969382478693</v>
       </c>
-      <c r="NF29" s="14" t="s">
-        <v>51</v>
+      <c r="NF29" s="11">
+        <v>54.76832783262</v>
       </c>
       <c r="NG29" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH29" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI29" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ29" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK29" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL29" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM29" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN29" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B30" s="12">
         <v>73.778714563351</v>
@@ -29913,39 +29944,39 @@
         <v>82.052720546437</v>
       </c>
       <c r="NE30" s="12">
-        <v>77.431767017449</v>
-      </c>
-      <c r="NF30" s="15" t="s">
-        <v>51</v>
+        <v>77.405844782974</v>
+      </c>
+      <c r="NF30" s="12">
+        <v>78.103332417306</v>
       </c>
       <c r="NG30" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH30" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI30" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ30" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK30" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL30" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM30" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN30" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B31" s="11">
         <v>73.811018646336</v>
@@ -30128,7 +30159,7 @@
         <v>92.530672204995</v>
       </c>
       <c r="BJ31" s="11">
-        <v>84.822315953759</v>
+        <v>84.822315953758</v>
       </c>
       <c r="BK31" s="11">
         <v>91.197770456276</v>
@@ -31049,39 +31080,39 @@
         <v>123.930523132745</v>
       </c>
       <c r="NE31" s="11">
-        <v>126.591375619751</v>
-      </c>
-      <c r="NF31" s="14" t="s">
-        <v>51</v>
+        <v>126.609956206852</v>
+      </c>
+      <c r="NF31" s="11">
+        <v>127.737968993687</v>
       </c>
       <c r="NG31" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH31" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI31" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ31" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK31" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL31" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM31" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN31" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B32" s="12">
         <v>86.120032958035</v>
@@ -32185,39 +32216,39 @@
         <v>120.846536399751</v>
       </c>
       <c r="NE32" s="12">
-        <v>114.47289932209</v>
-      </c>
-      <c r="NF32" s="15" t="s">
-        <v>51</v>
+        <v>114.545869535418</v>
+      </c>
+      <c r="NF32" s="12">
+        <v>113.578060380645</v>
       </c>
       <c r="NG32" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH32" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI32" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ32" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK32" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL32" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM32" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN32" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B33" s="11">
         <v>69.399412813085</v>
@@ -33321,39 +33352,39 @@
         <v>102.843824222956</v>
       </c>
       <c r="NE33" s="11">
-        <v>99.360726982542</v>
-      </c>
-      <c r="NF33" s="14" t="s">
-        <v>51</v>
+        <v>99.491181251437</v>
+      </c>
+      <c r="NF33" s="11">
+        <v>103.028452676052</v>
       </c>
       <c r="NG33" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH33" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI33" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ33" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK33" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL33" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM33" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN33" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B34" s="12">
         <v>72.622901666126</v>
@@ -34457,39 +34488,39 @@
         <v>124.059377651231</v>
       </c>
       <c r="NE34" s="12">
-        <v>110.683830820724</v>
-      </c>
-      <c r="NF34" s="15" t="s">
-        <v>51</v>
+        <v>110.358197023969</v>
+      </c>
+      <c r="NF34" s="12">
+        <v>110.539200147134</v>
       </c>
       <c r="NG34" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH34" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI34" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ34" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK34" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL34" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM34" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN34" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B35" s="11">
         <v>60.182989506094</v>
@@ -35593,39 +35624,39 @@
         <v>116.593168105942</v>
       </c>
       <c r="NE35" s="11">
-        <v>109.847219655183</v>
-      </c>
-      <c r="NF35" s="14" t="s">
-        <v>51</v>
+        <v>109.907144290227</v>
+      </c>
+      <c r="NF35" s="11">
+        <v>104.132272376595</v>
       </c>
       <c r="NG35" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH35" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI35" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ35" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK35" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL35" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM35" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN35" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B36" s="12">
         <v>61.132998870046</v>
@@ -36729,39 +36760,39 @@
         <v>151.886953168357</v>
       </c>
       <c r="NE36" s="12">
-        <v>139.395620149147</v>
-      </c>
-      <c r="NF36" s="15" t="s">
-        <v>51</v>
+        <v>139.391188901186</v>
+      </c>
+      <c r="NF36" s="12">
+        <v>139.952195088241</v>
       </c>
       <c r="NG36" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH36" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI36" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ36" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK36" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL36" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM36" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN36" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B37" s="11">
         <v>65.758484330262</v>
@@ -37865,39 +37896,39 @@
         <v>141.407793014073</v>
       </c>
       <c r="NE37" s="11">
-        <v>139.180788588841</v>
-      </c>
-      <c r="NF37" s="14" t="s">
-        <v>51</v>
+        <v>138.638611536248</v>
+      </c>
+      <c r="NF37" s="11">
+        <v>134.758845400809</v>
       </c>
       <c r="NG37" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH37" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI37" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ37" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK37" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL37" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM37" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN37" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B38" s="12">
         <v>33.546378018984</v>
@@ -39001,39 +39032,39 @@
         <v>139.354329819995</v>
       </c>
       <c r="NE38" s="12">
-        <v>126.44222991451</v>
-      </c>
-      <c r="NF38" s="15" t="s">
-        <v>51</v>
+        <v>126.442217469314</v>
+      </c>
+      <c r="NF38" s="12">
+        <v>119.508412270607</v>
       </c>
       <c r="NG38" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH38" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI38" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ38" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK38" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL38" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM38" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN38" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="11">
         <v>113.328554079414</v>
@@ -40137,39 +40168,39 @@
         <v>93.717052700775</v>
       </c>
       <c r="NE39" s="11">
-        <v>72.589839628819</v>
-      </c>
-      <c r="NF39" s="14" t="s">
-        <v>51</v>
+        <v>72.578971377205</v>
+      </c>
+      <c r="NF39" s="11">
+        <v>97.746666439157</v>
       </c>
       <c r="NG39" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH39" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI39" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ39" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK39" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL39" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM39" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN39" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B40" s="12">
         <v>42.404526159595</v>
@@ -41273,49 +41304,49 @@
         <v>125.213406415957</v>
       </c>
       <c r="NE40" s="12">
-        <v>115.330289807305</v>
-      </c>
-      <c r="NF40" s="15" t="s">
-        <v>51</v>
+        <v>115.261161474036</v>
+      </c>
+      <c r="NF40" s="12">
+        <v>129.097289499172</v>
       </c>
       <c r="NG40" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NH40" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NI40" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NJ40" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NK40" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NL40" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NM40" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="NN40" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47">
@@ -41355,7 +41386,7 @@
     <mergeCell ref="A5:A6"/>
   </mergeCells>
   <headerFooter/>
-  <legacyDrawing r:id="Rd5a862cd3f9a4e26"/>
+  <legacyDrawing r:id="R6693386db1154f38"/>
 </worksheet>
 </file>
 
@@ -41372,106 +41403,106 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
credentials + db update
</commit_message>
<xml_diff>
--- a/DATA/actind.xlsx
+++ b/DATA/actind.xlsx
@@ -5,8 +5,8 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Tabulado" sheetId="1" r:id="Rd5c07da3cfb24d2a"/>
-    <sheet name="MetaInfo" sheetId="2" r:id="Rd6cf121c3cf34f23"/>
+    <sheet name="Tabulado" sheetId="1" r:id="Re089cb1b5dd64b37"/>
+    <sheet name="MetaInfo" sheetId="2" r:id="R7d5bae15f22b4256"/>
   </sheets>
 </workbook>
 </file>
@@ -46,7 +46,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">R. Cifras revisadas</t>
+          <t xml:space="preserve">P. Cifras preliminares</t>
         </d:r>
       </text>
     </comment>
@@ -57,7 +57,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">R. Cifras revisadas</t>
+          <t xml:space="preserve">P. Cifras preliminares</t>
         </d:r>
       </text>
     </comment>
@@ -68,7 +68,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">R. Cifras revisadas</t>
+          <t xml:space="preserve">P. Cifras preliminares</t>
         </d:r>
       </text>
     </comment>
@@ -79,7 +79,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">R. Cifras revisadas</t>
+          <t xml:space="preserve">P. Cifras preliminares</t>
         </d:r>
       </text>
     </comment>
@@ -90,11 +90,22 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
+          <t xml:space="preserve">P. Cifras preliminares</t>
+        </d:r>
+      </text>
+    </comment>
+    <comment ref="NG6" authorId="0">
+      <text>
+        <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+          </rPr>
           <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
-    <comment ref="NG6" authorId="0">
+    <comment ref="NH6" authorId="0">
       <text>
         <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
           <rPr>
@@ -115,7 +126,7 @@
     <t>Instituto Nacional de Estadística y Geografía (INEGI).</t>
   </si>
   <si>
-    <t>Sistema de Cuentas Nacionales de México. Indicador Mensual de la Actividad Industrial. Año Base 2013. Serie de enero de 1993 a junio de 2021</t>
+    <t>Sistema de Cuentas Nacionales de México. Indicador Mensual de la Actividad Industrial. Año Base 2013. Serie de enero de 1993 a julio de 2021</t>
   </si>
   <si>
     <t>Índice de volumen físico base 2013=100</t>
@@ -300,7 +311,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">R</d:t>
+      <d:t xml:space="preserve">P</d:t>
     </d:r>
   </si>
   <si>
@@ -320,7 +331,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">R</d:t>
+      <d:t xml:space="preserve">P</d:t>
     </d:r>
   </si>
   <si>
@@ -340,7 +351,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">R</d:t>
+      <d:t xml:space="preserve">P</d:t>
     </d:r>
   </si>
   <si>
@@ -360,7 +371,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">R</d:t>
+      <d:t xml:space="preserve">P</d:t>
     </d:r>
   </si>
   <si>
@@ -380,6 +391,26 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
+      <d:t xml:space="preserve">P</d:t>
+    </d:r>
+  </si>
+  <si>
+    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:rPr>
+        <d:b/>
+        <d:sz val="10"/>
+        <d:rFont val="Calibri"/>
+      </d:rPr>
+      <d:t> Junio</d:t>
+    </d:r>
+    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:rPr>
+        <d:b/>
+        <d:vertAlign val="superscript"/>
+        <d:sz val="11"/>
+        <d:color rgb="FF000000"/>
+        <d:rFont val="Arial"/>
+      </d:rPr>
       <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
@@ -390,7 +421,7 @@
         <d:sz val="10"/>
         <d:rFont val="Calibri"/>
       </d:rPr>
-      <d:t> Junio</d:t>
+      <d:t> Julio</d:t>
     </d:r>
     <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <d:rPr>
@@ -547,9 +578,6 @@
     </d:r>
   </si>
   <si>
-    <t>Nota: Con base en los ´´Lineamientos de cambios a la información divulgada en las publicaciones estadísticas y geográficas del INEGI´´ y que complementan las ´´Normas Especiales para la Divulgación de Datos´´ del FMI, los resultados del Indicador Mensual de la Actividad Industrial incorporan la última información estadística disponible de la Estadística de la Industria Minerometalúrgica, la Encuesta Nacional de Empresas Constructoras, la Encuesta Mensual de la Industria Manufacturera, los registros administrativos y los datos primarios del año 2021, por lo que se debe actualizar el indicador. Como resultado de incorporar dicha información, se identifican diferencias en los niveles de los índices y variaciones que fueron oportunamente publicadas.</t>
-  </si>
-  <si>
     <t>Fuente: INEGI. Sistema de Cuentas Nacionales de México. Indicador Mensual de la Actividad Industrial</t>
   </si>
   <si>
@@ -616,19 +644,19 @@
     <t>COBERTURA TEMPORAL</t>
   </si>
   <si>
-    <t>1993-01-2021-06</t>
+    <t>1993-01-2021-07</t>
   </si>
   <si>
     <t>DESCRIPCIÓN PERIODO</t>
   </si>
   <si>
-    <t>Serie de enero de 1993 a junio de 2021</t>
+    <t>Serie de enero de 1993 a julio de 2021</t>
   </si>
   <si>
     <t>FECHA DE ACTUALIZACIÓN</t>
   </si>
   <si>
-    <t>2021-08-11</t>
+    <t>2021-09-10</t>
   </si>
 </sst>
 </file>
@@ -769,7 +797,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:NN48"/>
+  <dimension ref="A1:NN47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2723,7 +2751,7 @@
         <v>51</v>
       </c>
       <c r="NH6" s="10" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="NI6" s="10" t="s">
         <v>40</v>
@@ -2746,7 +2774,7 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="11">
         <v>69.222752741001</v>
@@ -3856,33 +3884,33 @@
         <v>98.610058992661</v>
       </c>
       <c r="NG7" s="11">
-        <v>97.756083895029</v>
-      </c>
-      <c r="NH7" s="14" t="s">
-        <v>53</v>
+        <v>97.719139242435</v>
+      </c>
+      <c r="NH7" s="11">
+        <v>98.251685818355</v>
       </c>
       <c r="NI7" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ7" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK7" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL7" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM7" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN7" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B8" s="12">
         <v>85.987958716261</v>
@@ -4992,33 +5020,33 @@
         <v>75.993360509255</v>
       </c>
       <c r="NG8" s="12">
-        <v>73.532983832429</v>
-      </c>
-      <c r="NH8" s="15" t="s">
-        <v>53</v>
+        <v>73.442879869386</v>
+      </c>
+      <c r="NH8" s="12">
+        <v>72.895857004091</v>
       </c>
       <c r="NI8" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ8" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK8" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL8" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM8" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN8" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B9" s="11">
         <v>99.519341749343</v>
@@ -6130,31 +6158,31 @@
       <c r="NG9" s="11">
         <v>65.971109230481</v>
       </c>
-      <c r="NH9" s="14" t="s">
-        <v>53</v>
+      <c r="NH9" s="11">
+        <v>67.747174467944</v>
       </c>
       <c r="NI9" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ9" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK9" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL9" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM9" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN9" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B10" s="12">
         <v>48.814950253715</v>
@@ -7264,33 +7292,33 @@
         <v>107.08072000644</v>
       </c>
       <c r="NG10" s="12">
-        <v>102.986395502164</v>
-      </c>
-      <c r="NH10" s="15" t="s">
-        <v>53</v>
+        <v>102.397934755908</v>
+      </c>
+      <c r="NH10" s="12">
+        <v>103.922587658415</v>
       </c>
       <c r="NI10" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ10" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK10" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL10" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM10" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN10" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" s="11">
         <v>22.744141472693</v>
@@ -8400,33 +8428,33 @@
         <v>89.42984354167</v>
       </c>
       <c r="NG11" s="11">
-        <v>93.005517188237</v>
-      </c>
-      <c r="NH11" s="14" t="s">
-        <v>53</v>
+        <v>92.952911166371</v>
+      </c>
+      <c r="NH11" s="11">
+        <v>66.09082401142</v>
       </c>
       <c r="NI11" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ11" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK11" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL11" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM11" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN11" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B12" s="12">
         <v>38.665943249786</v>
@@ -8951,7 +8979,7 @@
         <v>82.285700021575</v>
       </c>
       <c r="FT12" s="12">
-        <v>84.872908092727</v>
+        <v>84.872908092728</v>
       </c>
       <c r="FU12" s="12">
         <v>87.006771936463</v>
@@ -9536,33 +9564,33 @@
         <v>112.266280021283</v>
       </c>
       <c r="NG12" s="12">
-        <v>115.24508616476</v>
-      </c>
-      <c r="NH12" s="15" t="s">
-        <v>53</v>
+        <v>115.11939157212</v>
+      </c>
+      <c r="NH12" s="12">
+        <v>119.325491368361</v>
       </c>
       <c r="NI12" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ12" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK12" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL12" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM12" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN12" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B13" s="11">
         <v>33.532463105934</v>
@@ -10087,7 +10115,7 @@
         <v>77.96308232892</v>
       </c>
       <c r="FT13" s="11">
-        <v>81.350354205881</v>
+        <v>81.350354205882</v>
       </c>
       <c r="FU13" s="11">
         <v>83.983953249091</v>
@@ -10672,33 +10700,33 @@
         <v>113.520849351763</v>
       </c>
       <c r="NG13" s="11">
-        <v>117.269274323843</v>
-      </c>
-      <c r="NH13" s="14" t="s">
-        <v>53</v>
+        <v>117.106972340176</v>
+      </c>
+      <c r="NH13" s="11">
+        <v>123.143109517566</v>
       </c>
       <c r="NI13" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ13" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK13" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL13" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM13" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN13" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B14" s="12">
         <v>56.292184219235</v>
@@ -11810,31 +11838,31 @@
       <c r="NG14" s="12">
         <v>108.294863847795</v>
       </c>
-      <c r="NH14" s="15" t="s">
-        <v>53</v>
+      <c r="NH14" s="12">
+        <v>106.217374546712</v>
       </c>
       <c r="NI14" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ14" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK14" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL14" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM14" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN14" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B15" s="11">
         <v>71.2627077305</v>
@@ -12944,33 +12972,33 @@
         <v>90.169849220607</v>
       </c>
       <c r="NG15" s="11">
-        <v>86.062428792484</v>
-      </c>
-      <c r="NH15" s="14" t="s">
-        <v>53</v>
+        <v>85.933624418293</v>
+      </c>
+      <c r="NH15" s="11">
+        <v>88.209969178939</v>
       </c>
       <c r="NI15" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ15" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK15" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL15" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM15" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN15" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B16" s="12">
         <v>84.037802362945</v>
@@ -13864,7 +13892,7 @@
         <v>107.456876229305</v>
       </c>
       <c r="KM16" s="12">
-        <v>109.69972489064</v>
+        <v>109.699724890639</v>
       </c>
       <c r="KN16" s="12">
         <v>106.221231756916</v>
@@ -14080,33 +14108,33 @@
         <v>99.463672205599</v>
       </c>
       <c r="NG16" s="12">
-        <v>91.042553613982</v>
-      </c>
-      <c r="NH16" s="15" t="s">
-        <v>53</v>
+        <v>90.797806764448</v>
+      </c>
+      <c r="NH16" s="12">
+        <v>94.041152620565</v>
       </c>
       <c r="NI16" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ16" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK16" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL16" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM16" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN16" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B17" s="11">
         <v>35.064527007042</v>
@@ -15183,7 +15211,7 @@
         <v>50.631944025606</v>
       </c>
       <c r="MV17" s="11">
-        <v>56.073389775793</v>
+        <v>56.073389775792</v>
       </c>
       <c r="MW17" s="11">
         <v>53.730057240421</v>
@@ -15216,33 +15244,33 @@
         <v>51.992871526456</v>
       </c>
       <c r="NG17" s="11">
-        <v>50.698025773277</v>
-      </c>
-      <c r="NH17" s="14" t="s">
-        <v>53</v>
+        <v>50.791743509044</v>
+      </c>
+      <c r="NH17" s="11">
+        <v>56.422069954497</v>
       </c>
       <c r="NI17" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ17" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK17" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL17" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM17" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN17" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B18" s="12">
         <v>73.87209194618</v>
@@ -16352,33 +16380,33 @@
         <v>118.116987550032</v>
       </c>
       <c r="NG18" s="12">
-        <v>133.826537399665</v>
-      </c>
-      <c r="NH18" s="15" t="s">
-        <v>53</v>
+        <v>133.907201052341</v>
+      </c>
+      <c r="NH18" s="12">
+        <v>122.977249738745</v>
       </c>
       <c r="NI18" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ18" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK18" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL18" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM18" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN18" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B19" s="11">
         <v>63.653052579688</v>
@@ -17215,7 +17243,7 @@
         <v>106.941322006685</v>
       </c>
       <c r="JT19" s="11">
-        <v>105.230620689974</v>
+        <v>105.230620689975</v>
       </c>
       <c r="JU19" s="11">
         <v>105.554969592329</v>
@@ -17263,7 +17291,7 @@
         <v>107.711396263853</v>
       </c>
       <c r="KJ19" s="11">
-        <v>108.022283783149</v>
+        <v>108.022283783148</v>
       </c>
       <c r="KK19" s="11">
         <v>113.751953282089</v>
@@ -17488,33 +17516,33 @@
         <v>111.406634279482</v>
       </c>
       <c r="NG19" s="11">
-        <v>112.437318933241</v>
-      </c>
-      <c r="NH19" s="14" t="s">
-        <v>53</v>
+        <v>112.4757329322</v>
+      </c>
+      <c r="NH19" s="11">
+        <v>112.324409153513</v>
       </c>
       <c r="NI19" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ19" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK19" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL19" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM19" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN19" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B20" s="12">
         <v>63.907698868213</v>
@@ -18624,33 +18652,33 @@
         <v>117.302674602582</v>
       </c>
       <c r="NG20" s="12">
-        <v>116.493719750459</v>
-      </c>
-      <c r="NH20" s="15" t="s">
-        <v>53</v>
+        <v>116.496153530384</v>
+      </c>
+      <c r="NH20" s="12">
+        <v>116.043575309129</v>
       </c>
       <c r="NI20" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ20" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK20" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL20" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM20" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN20" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B21" s="11">
         <v>56.569385260854</v>
@@ -19760,33 +19788,33 @@
         <v>131.026131943119</v>
       </c>
       <c r="NG21" s="11">
-        <v>134.455722871202</v>
-      </c>
-      <c r="NH21" s="14" t="s">
-        <v>53</v>
+        <v>134.455671698255</v>
+      </c>
+      <c r="NH21" s="11">
+        <v>138.990993597344</v>
       </c>
       <c r="NI21" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ21" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK21" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL21" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM21" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN21" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B22" s="12">
         <v>114.319677175604</v>
@@ -20212,7 +20240,7 @@
         <v>117.907452401807</v>
       </c>
       <c r="EM22" s="12">
-        <v>102.663934277922</v>
+        <v>102.663934277921</v>
       </c>
       <c r="EN22" s="12">
         <v>121.171668236243</v>
@@ -20898,31 +20926,31 @@
       <c r="NG22" s="12">
         <v>94.139234170372</v>
       </c>
-      <c r="NH22" s="15" t="s">
-        <v>53</v>
+      <c r="NH22" s="12">
+        <v>95.115092548317</v>
       </c>
       <c r="NI22" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ22" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK22" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL22" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM22" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN22" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B23" s="11">
         <v>120.050850501477</v>
@@ -21642,7 +21670,7 @@
         <v>93.175225480757</v>
       </c>
       <c r="IG23" s="11">
-        <v>96.070279662976</v>
+        <v>96.070279662975</v>
       </c>
       <c r="IH23" s="11">
         <v>101.737313361619</v>
@@ -22032,33 +22060,33 @@
         <v>103.582434438996</v>
       </c>
       <c r="NG23" s="11">
-        <v>102.537187503302</v>
-      </c>
-      <c r="NH23" s="14" t="s">
-        <v>53</v>
+        <v>102.442158450718</v>
+      </c>
+      <c r="NH23" s="11">
+        <v>109.419610214933</v>
       </c>
       <c r="NI23" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ23" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK23" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL23" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM23" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN23" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B24" s="12">
         <v>90.688383871069</v>
@@ -23168,33 +23196,33 @@
         <v>84.623253840156</v>
       </c>
       <c r="NG24" s="12">
-        <v>82.065978857869</v>
-      </c>
-      <c r="NH24" s="15" t="s">
-        <v>53</v>
+        <v>82.092782073871</v>
+      </c>
+      <c r="NH24" s="12">
+        <v>80.066902874358</v>
       </c>
       <c r="NI24" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ24" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK24" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL24" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM24" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN24" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B25" s="11">
         <v>139.460849924193</v>
@@ -24306,31 +24334,31 @@
       <c r="NG25" s="11">
         <v>74.611041644678</v>
       </c>
-      <c r="NH25" s="14" t="s">
-        <v>53</v>
+      <c r="NH25" s="11">
+        <v>74.889378232599</v>
       </c>
       <c r="NI25" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ25" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK25" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL25" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM25" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN25" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B26" s="12">
         <v>130.395494603712</v>
@@ -25092,7 +25120,7 @@
         <v>111.318450734813</v>
       </c>
       <c r="IU26" s="12">
-        <v>97.416158126745</v>
+        <v>97.416158126744</v>
       </c>
       <c r="IV26" s="12">
         <v>107.114454959646</v>
@@ -25440,33 +25468,33 @@
         <v>96.385404863874</v>
       </c>
       <c r="NG26" s="12">
-        <v>107.465012685658</v>
-      </c>
-      <c r="NH26" s="15" t="s">
-        <v>53</v>
+        <v>107.950441508887</v>
+      </c>
+      <c r="NH26" s="12">
+        <v>106.388737803037</v>
       </c>
       <c r="NI26" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ26" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK26" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL26" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM26" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN26" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B27" s="11">
         <v>51.479382699588</v>
@@ -26576,33 +26604,33 @@
         <v>131.041141157866</v>
       </c>
       <c r="NG27" s="11">
-        <v>122.906913612617</v>
-      </c>
-      <c r="NH27" s="14" t="s">
-        <v>53</v>
+        <v>122.900860636101</v>
+      </c>
+      <c r="NH27" s="11">
+        <v>126.165419939631</v>
       </c>
       <c r="NI27" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ27" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK27" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL27" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM27" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN27" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B28" s="12">
         <v>68.358361009475</v>
@@ -27712,33 +27740,33 @@
         <v>101.342666356018</v>
       </c>
       <c r="NG28" s="12">
-        <v>110.086413440673</v>
-      </c>
-      <c r="NH28" s="15" t="s">
-        <v>53</v>
+        <v>109.9806808482</v>
+      </c>
+      <c r="NH28" s="12">
+        <v>109.802876137791</v>
       </c>
       <c r="NI28" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ28" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK28" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL28" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM28" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN28" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B29" s="11">
         <v>76.901717312341</v>
@@ -28848,33 +28876,33 @@
         <v>54.710091472634</v>
       </c>
       <c r="NG29" s="11">
-        <v>47.628670412601</v>
-      </c>
-      <c r="NH29" s="14" t="s">
-        <v>53</v>
+        <v>47.504338860699</v>
+      </c>
+      <c r="NH29" s="11">
+        <v>52.45003839176</v>
       </c>
       <c r="NI29" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ29" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK29" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL29" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM29" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN29" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B30" s="12">
         <v>73.778714563351</v>
@@ -29984,33 +30012,33 @@
         <v>78.351268967003</v>
       </c>
       <c r="NG30" s="12">
-        <v>79.717583771148</v>
-      </c>
-      <c r="NH30" s="15" t="s">
-        <v>53</v>
+        <v>80.140220111041</v>
+      </c>
+      <c r="NH30" s="12">
+        <v>85.298202174664</v>
       </c>
       <c r="NI30" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ30" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK30" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL30" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM30" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN30" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B31" s="11">
         <v>73.811018646336</v>
@@ -30193,7 +30221,7 @@
         <v>92.530672204995</v>
       </c>
       <c r="BJ31" s="11">
-        <v>84.822315953758</v>
+        <v>84.822315953759</v>
       </c>
       <c r="BK31" s="11">
         <v>91.197770456276</v>
@@ -30814,7 +30842,7 @@
         <v>105.279540530588</v>
       </c>
       <c r="JI31" s="11">
-        <v>103.79997342929</v>
+        <v>103.799973429289</v>
       </c>
       <c r="JJ31" s="11">
         <v>97.719773098197</v>
@@ -31120,33 +31148,33 @@
         <v>127.916901116271</v>
       </c>
       <c r="NG31" s="11">
-        <v>130.416157403404</v>
-      </c>
-      <c r="NH31" s="14" t="s">
-        <v>53</v>
+        <v>130.461764866534</v>
+      </c>
+      <c r="NH31" s="11">
+        <v>129.832182715271</v>
       </c>
       <c r="NI31" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ31" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK31" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL31" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM31" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN31" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B32" s="12">
         <v>86.120032958035</v>
@@ -32256,33 +32284,33 @@
         <v>113.7614698419</v>
       </c>
       <c r="NG32" s="12">
-        <v>114.837505804048</v>
-      </c>
-      <c r="NH32" s="15" t="s">
-        <v>53</v>
+        <v>114.849895122055</v>
+      </c>
+      <c r="NH32" s="12">
+        <v>120.317941542966</v>
       </c>
       <c r="NI32" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ32" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK32" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL32" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM32" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN32" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B33" s="11">
         <v>69.399412813085</v>
@@ -33394,31 +33422,31 @@
       <c r="NG33" s="11">
         <v>97.313792928414</v>
       </c>
-      <c r="NH33" s="14" t="s">
-        <v>53</v>
+      <c r="NH33" s="11">
+        <v>97.561659430102</v>
       </c>
       <c r="NI33" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ33" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK33" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL33" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM33" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN33" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B34" s="12">
         <v>72.622901666126</v>
@@ -33991,7 +34019,7 @@
         <v>116.458896659146</v>
       </c>
       <c r="GJ34" s="12">
-        <v>107.179010492019</v>
+        <v>107.179010492018</v>
       </c>
       <c r="GK34" s="12">
         <v>115.46329954894</v>
@@ -34030,7 +34058,7 @@
         <v>107.220124251125</v>
       </c>
       <c r="GW34" s="12">
-        <v>105.452330853942</v>
+        <v>105.452330853943</v>
       </c>
       <c r="GX34" s="12">
         <v>115.02590334585</v>
@@ -34222,7 +34250,7 @@
         <v>101.595831692184</v>
       </c>
       <c r="JI34" s="12">
-        <v>101.467953672713</v>
+        <v>101.467953672712</v>
       </c>
       <c r="JJ34" s="12">
         <v>97.944257143157</v>
@@ -34318,7 +34346,7 @@
         <v>109.976767217928</v>
       </c>
       <c r="KO34" s="12">
-        <v>107.874867879491</v>
+        <v>107.87486787949</v>
       </c>
       <c r="KP34" s="12">
         <v>112.689978501788</v>
@@ -34528,33 +34556,33 @@
         <v>110.5554692786</v>
       </c>
       <c r="NG34" s="12">
-        <v>112.474052484218</v>
-      </c>
-      <c r="NH34" s="15" t="s">
-        <v>53</v>
+        <v>112.47579611705</v>
+      </c>
+      <c r="NH34" s="12">
+        <v>114.467948972667</v>
       </c>
       <c r="NI34" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ34" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK34" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL34" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM34" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN34" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B35" s="11">
         <v>60.182989506094</v>
@@ -35664,33 +35692,33 @@
         <v>104.206148656917</v>
       </c>
       <c r="NG35" s="11">
-        <v>110.820488051284</v>
-      </c>
-      <c r="NH35" s="14" t="s">
-        <v>53</v>
+        <v>110.826570815905</v>
+      </c>
+      <c r="NH35" s="11">
+        <v>104.866820173805</v>
       </c>
       <c r="NI35" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ35" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK35" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL35" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM35" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN35" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B36" s="12">
         <v>61.132998870046</v>
@@ -36260,7 +36288,7 @@
         <v>107.863814613867</v>
       </c>
       <c r="GI36" s="12">
-        <v>126.09453857615</v>
+        <v>126.094538576149</v>
       </c>
       <c r="GJ36" s="12">
         <v>125.489105446636</v>
@@ -36281,7 +36309,7 @@
         <v>112.53675029352</v>
       </c>
       <c r="GP36" s="12">
-        <v>105.708098106801</v>
+        <v>105.708098106802</v>
       </c>
       <c r="GQ36" s="12">
         <v>110.211745409613</v>
@@ -36802,31 +36830,31 @@
       <c r="NG36" s="12">
         <v>137.177928999875</v>
       </c>
-      <c r="NH36" s="15" t="s">
-        <v>53</v>
+      <c r="NH36" s="12">
+        <v>144.406971792021</v>
       </c>
       <c r="NI36" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ36" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK36" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL36" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM36" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN36" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B37" s="11">
         <v>65.758484330262</v>
@@ -37225,7 +37253,7 @@
         <v>109.375136947249</v>
       </c>
       <c r="ED37" s="11">
-        <v>103.630122854371</v>
+        <v>103.630122854372</v>
       </c>
       <c r="EE37" s="11">
         <v>95.918036976017</v>
@@ -37612,7 +37640,7 @@
         <v>100.808222495904</v>
       </c>
       <c r="JC37" s="11">
-        <v>98.353856914581</v>
+        <v>98.35385691458</v>
       </c>
       <c r="JD37" s="11">
         <v>94.616077569601</v>
@@ -37804,7 +37832,7 @@
         <v>117.339402188725</v>
       </c>
       <c r="LO37" s="11">
-        <v>111.243619478106</v>
+        <v>111.243619478105</v>
       </c>
       <c r="LP37" s="11">
         <v>113.05386535961</v>
@@ -37938,31 +37966,31 @@
       <c r="NG37" s="11">
         <v>140.832381978733</v>
       </c>
-      <c r="NH37" s="14" t="s">
-        <v>53</v>
+      <c r="NH37" s="11">
+        <v>141.030669167153</v>
       </c>
       <c r="NI37" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ37" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK37" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL37" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM37" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN37" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B38" s="12">
         <v>33.546378018984</v>
@@ -39072,33 +39100,33 @@
         <v>119.507718595814</v>
       </c>
       <c r="NG38" s="12">
-        <v>126.314569714816</v>
-      </c>
-      <c r="NH38" s="15" t="s">
-        <v>53</v>
+        <v>126.319873438929</v>
+      </c>
+      <c r="NH38" s="12">
+        <v>116.799082308144</v>
       </c>
       <c r="NI38" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ38" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK38" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL38" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM38" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN38" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B39" s="11">
         <v>113.328554079414</v>
@@ -40058,7 +40086,7 @@
         <v>88.455549785448</v>
       </c>
       <c r="LI39" s="11">
-        <v>90.391653887423</v>
+        <v>90.391653887422</v>
       </c>
       <c r="LJ39" s="11">
         <v>94.579359088044</v>
@@ -40208,33 +40236,33 @@
         <v>97.703130456019</v>
       </c>
       <c r="NG39" s="11">
-        <v>98.853068480946</v>
-      </c>
-      <c r="NH39" s="14" t="s">
-        <v>53</v>
+        <v>98.853691730342</v>
+      </c>
+      <c r="NH39" s="11">
+        <v>93.253079011255</v>
       </c>
       <c r="NI39" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ39" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK39" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL39" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM39" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN39" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B40" s="12">
         <v>42.404526159595</v>
@@ -41041,7 +41069,7 @@
         <v>100.047769469755</v>
       </c>
       <c r="JJ40" s="12">
-        <v>98.265948470573</v>
+        <v>98.265948470574</v>
       </c>
       <c r="JK40" s="12">
         <v>111.175398244536</v>
@@ -41344,52 +41372,47 @@
         <v>129.095442746663</v>
       </c>
       <c r="NG40" s="12">
-        <v>123.575923754268</v>
-      </c>
-      <c r="NH40" s="15" t="s">
-        <v>53</v>
+        <v>123.12030063746</v>
+      </c>
+      <c r="NH40" s="12">
+        <v>133.788904951557</v>
       </c>
       <c r="NI40" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NJ40" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NK40" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NL40" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NM40" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="NN40" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="3"/>
+      <c r="A47" s="3"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -41425,7 +41448,7 @@
     <mergeCell ref="A5:A6"/>
   </mergeCells>
   <headerFooter/>
-  <legacyDrawing r:id="Re86338461a2d478f"/>
+  <legacyDrawing r:id="R3bd3e29c36bb409b"/>
 </worksheet>
 </file>
 

</xml_diff>